<commit_message>
uc06 - revisão completa
</commit_message>
<xml_diff>
--- a/Sprint 2/UC06_Especificar_Tarefa/UC6_TestScenario.xlsx
+++ b/Sprint 2/UC06_Especificar_Tarefa/UC6_TestScenario.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05A2B640-E044-4A9F-86B1-8C9DB03E5D7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blest\Desktop\Sprints\upskill_java1_labprg_grupo2\Sprint 2\UC06_Especificar_Tarefa\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591E84A9-C065-45F9-9901-BA2B1E0549E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="2955" windowWidth="20730" windowHeight="11160" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Mover ficheiro" sheetId="2" r:id="rId2"/>
     <sheet name="Cancelar encomenda" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="96">
   <si>
     <t>Project Name</t>
   </si>
@@ -416,12 +421,21 @@
   <si>
     <t>Cancelar encomenda que não é reembolsável</t>
   </si>
+  <si>
+    <t>T4J - Sprint 2</t>
+  </si>
+  <si>
+    <t>Ana Batista</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -479,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -494,6 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,7 +596,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -879,56 +894,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.75"/>
     <col min="2" max="2" width="24" style="1"/>
     <col min="3" max="4" width="24"/>
-    <col min="5" max="9" width="24.125" customWidth="1"/>
-    <col min="10" max="1025" width="10.875"/>
+    <col min="5" max="9" width="24.08203125" customWidth="1"/>
+    <col min="10" max="1025" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="B5" s="6">
+        <v>44225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -957,7 +978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="31.5">
+    <row r="9" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -986,7 +1007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1015,7 +1036,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="5" customFormat="1" ht="162.75" customHeight="1">
+    <row r="11" spans="1:9" s="5" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1044,7 +1065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="5" customFormat="1" ht="280.5" customHeight="1">
+    <row r="12" spans="1:9" s="5" customFormat="1" ht="280.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1073,7 +1094,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.100000000000001">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -1102,7 +1123,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="5" customFormat="1" ht="173.25">
+    <row r="14" spans="1:9" s="5" customFormat="1" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1131,7 +1152,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="5" customFormat="1" ht="63">
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -1160,7 +1181,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" ht="63">
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -1189,13 +1210,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B17"/>
     </row>
-    <row r="18" spans="1:9" ht="17.100000000000001">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
@@ -1224,24 +1245,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1253,51 +1274,51 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.75"/>
     <col min="2" max="2" width="24" style="1"/>
     <col min="3" max="5" width="24"/>
-    <col min="6" max="1025" width="10.875"/>
+    <col min="6" max="1025" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="8" spans="1:5" ht="17.100000000000001">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1314,7 +1335,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="33.950000000000003">
+    <row r="9" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1331,7 +1352,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.100000000000001">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1348,7 +1369,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="51">
+    <row r="11" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1365,7 +1386,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="33.950000000000003">
+    <row r="12" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -1382,7 +1403,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="33.950000000000003">
+    <row r="13" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -1399,7 +1420,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="33.950000000000003">
+    <row r="14" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1416,7 +1437,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="51">
+    <row r="15" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1433,7 +1454,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="51">
+    <row r="16" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
@@ -1450,13 +1471,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B17"/>
     </row>
-    <row r="18" spans="1:5" ht="17.100000000000001">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
@@ -1473,24 +1494,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -1502,51 +1523,51 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.75"/>
     <col min="2" max="2" width="24" style="1"/>
     <col min="3" max="5" width="24"/>
-    <col min="6" max="1025" width="10.875"/>
+    <col min="6" max="1025" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="8" spans="1:5" ht="17.100000000000001">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1563,7 +1584,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="51">
+    <row r="9" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1580,7 +1601,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1588,7 +1609,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1596,7 +1617,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -1604,7 +1625,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -1612,7 +1633,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1620,7 +1641,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1628,7 +1649,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
@@ -1636,12 +1657,12 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
@@ -1649,23 +1670,23 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>